<commit_message>
VCF-4P - BOM update
</commit_message>
<xml_diff>
--- a/modules/VCF-4P/VCF-4P-BOM.xlsx
+++ b/modules/VCF-4P/VCF-4P-BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Len\Documents\Dev\git\Synth-priv\modules\VCF-4P\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\VCF-4P\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400AECE5-CDED-4262-8324-3102A9E74B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4DF2ABE-09BE-4986-817F-4DA6B03F2F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2985" yWindow="1785" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VCF-4P-BOM" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="211">
   <si>
     <t>Ref</t>
   </si>
@@ -223,18 +223,12 @@
     <t>https://www.mouser.ca/ProductDetail/Panasonic/ECE-A1EN100UI?qs=0h1gzos03f36mGOUyzNXaA%3D%3D</t>
   </si>
   <si>
-    <t>H5 H7 H8 H10</t>
-  </si>
-  <si>
     <t>M3x0.50x6</t>
   </si>
   <si>
     <t>Machine screw, M3x0.50x6</t>
   </si>
   <si>
-    <t>H6 H9</t>
-  </si>
-  <si>
     <t>11mm_M3x0.50</t>
   </si>
   <si>
@@ -262,9 +256,6 @@
     <t>https://www.mouser.ca/ProductDetail/Wurth-Elektronik/970110321?qs=wr8lucFkNMUs0IWSCWTB3w%3D%3D</t>
   </si>
   <si>
-    <t>H11</t>
-  </si>
-  <si>
     <t>Jumper_2</t>
   </si>
   <si>
@@ -286,9 +277,6 @@
     <t>https://www.adafruit.com/product/3525</t>
   </si>
   <si>
-    <t>J1 J3 J4 J5 J7</t>
-  </si>
-  <si>
     <t>WQP-PJ398</t>
   </si>
   <si>
@@ -478,9 +466,6 @@
     <t>https://www.mouser.ca/ProductDetail/Vishay-Dale/CCF071K00JKE36?qs=sGAEpiMZZMsPqMdJzcrNwqw41JD0NFylHV1MADcQnpo%3D</t>
   </si>
   <si>
-    <t>RV1 RV6</t>
-  </si>
-  <si>
     <t>LIN</t>
   </si>
   <si>
@@ -514,15 +499,9 @@
     <t>https://synthcube.com/cart/alpha-9mm-potentiometer-right-angle-pcb-mount-6-35mm-round-shaft</t>
   </si>
   <si>
-    <t>RV3</t>
-  </si>
-  <si>
     <t>LOG</t>
   </si>
   <si>
-    <t>RV4 RV8</t>
-  </si>
-  <si>
     <t>http://www.song-huei.com/proimages//eng/pdfimages/R0904N.pdf</t>
   </si>
   <si>
@@ -635,6 +614,57 @@
   </si>
   <si>
     <t>Need</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>Delptronics_MCS_10HP</t>
+  </si>
+  <si>
+    <t>PCB &amp; panel kit</t>
+  </si>
+  <si>
+    <t>Delptronics Module Construction Set - 10HP PCB &amp; panel kit</t>
+  </si>
+  <si>
+    <t>https://delptronics.com/module-construction-set.php</t>
+  </si>
+  <si>
+    <t>Delptronics</t>
+  </si>
+  <si>
+    <t>synthCube</t>
+  </si>
+  <si>
+    <t>DELPMCSMSTR</t>
+  </si>
+  <si>
+    <t>https://synthcube.com/cart/delptronics-module-construction-set</t>
+  </si>
+  <si>
+    <t>https://modularaddict.com/module-construction-set-eurorack-prototype-development-platform-delptronics</t>
+  </si>
+  <si>
+    <t>H3 H4</t>
+  </si>
+  <si>
+    <t>H5</t>
+  </si>
+  <si>
+    <t>J1 J3 J5 J7 J8</t>
+  </si>
+  <si>
+    <t>RV1 RV7</t>
+  </si>
+  <si>
+    <t>RV2 RV8</t>
+  </si>
+  <si>
+    <t>RV4</t>
   </si>
 </sst>
 </file>
@@ -1166,7 +1196,17 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1487,18 +1527,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U31"/>
+  <dimension ref="A1:U32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="5" width="4.3984375" customWidth="1"/>
+    <col min="2" max="5" width="4.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1506,13 +1546,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -1563,7 +1603,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1605,7 +1645,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1616,7 +1656,7 @@
         <v>2</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E31" si="0">MAX(0,B3-C3-D3)</f>
+        <f t="shared" ref="E3:E32" si="0">MAX(0,B3-C3-D3)</f>
         <v>0</v>
       </c>
       <c r="F3" t="s">
@@ -1647,7 +1687,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1689,7 +1729,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -1731,7 +1771,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -1773,216 +1813,228 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>194</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f>MAX(0,B7-C7-D7)</f>
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="I7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+        <v>75</v>
+      </c>
+      <c r="J7" t="s">
+        <v>76</v>
+      </c>
+      <c r="M7" t="s">
+        <v>35</v>
+      </c>
+      <c r="N7" t="s">
+        <v>77</v>
+      </c>
+      <c r="O7" t="s">
+        <v>78</v>
+      </c>
+      <c r="P7" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q7">
+        <v>3525</v>
+      </c>
+      <c r="R7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>195</v>
       </c>
       <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <f>MAX(0,B8-C8-D8)</f>
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>196</v>
+      </c>
+      <c r="H8" t="s">
+        <v>197</v>
+      </c>
+      <c r="I8" t="s">
+        <v>198</v>
+      </c>
+      <c r="J8" t="s">
+        <v>199</v>
+      </c>
+      <c r="K8" t="s">
+        <v>200</v>
+      </c>
+      <c r="M8" t="s">
+        <v>200</v>
+      </c>
+      <c r="O8" t="s">
+        <v>199</v>
+      </c>
+      <c r="P8" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>202</v>
+      </c>
+      <c r="R8" t="s">
+        <v>203</v>
+      </c>
+      <c r="S8" t="s">
+        <v>26</v>
+      </c>
+      <c r="U8" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>205</v>
+      </c>
+      <c r="B9">
         <v>2</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>2</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>67</v>
-      </c>
-      <c r="I8" t="s">
-        <v>68</v>
-      </c>
-      <c r="J8" t="s">
-        <v>69</v>
-      </c>
-      <c r="K8" t="s">
-        <v>70</v>
-      </c>
-      <c r="L8" t="s">
-        <v>71</v>
-      </c>
-      <c r="M8" t="s">
-        <v>22</v>
-      </c>
-      <c r="N8" t="s">
-        <v>72</v>
-      </c>
-      <c r="O8" t="s">
-        <v>73</v>
-      </c>
-      <c r="P8" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>74</v>
-      </c>
-      <c r="R8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="I9" t="s">
-        <v>78</v>
-      </c>
-      <c r="J9" t="s">
-        <v>79</v>
-      </c>
-      <c r="M9" t="s">
-        <v>35</v>
-      </c>
-      <c r="N9" t="s">
-        <v>80</v>
-      </c>
-      <c r="O9" t="s">
-        <v>81</v>
-      </c>
-      <c r="P9" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q9">
-        <v>3525</v>
-      </c>
-      <c r="R9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>206</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="I10" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="J10" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="K10" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="L10" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="M10" t="s">
         <v>22</v>
       </c>
       <c r="N10" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="O10" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="P10" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="Q10" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="R10" t="s">
-        <v>93</v>
-      </c>
-      <c r="S10" t="s">
-        <v>82</v>
-      </c>
-      <c r="T10">
-        <v>4031</v>
-      </c>
-      <c r="U10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>207</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="I11" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="J11" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="K11" t="s">
-        <v>99</v>
-      </c>
-      <c r="L11">
-        <v>61201621621</v>
+        <v>84</v>
+      </c>
+      <c r="L11" t="s">
+        <v>85</v>
       </c>
       <c r="M11" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="N11" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="O11" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+        <v>87</v>
+      </c>
+      <c r="P11" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>88</v>
+      </c>
+      <c r="R11" t="s">
+        <v>89</v>
+      </c>
+      <c r="S11" t="s">
+        <v>79</v>
+      </c>
+      <c r="T11">
+        <v>4031</v>
+      </c>
+      <c r="U11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1995,15 +2047,33 @@
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="I12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+        <v>93</v>
+      </c>
+      <c r="J12" t="s">
+        <v>94</v>
+      </c>
+      <c r="K12" t="s">
+        <v>95</v>
+      </c>
+      <c r="L12">
+        <v>61201621621</v>
+      </c>
+      <c r="M12" t="s">
+        <v>35</v>
+      </c>
+      <c r="N12" t="s">
+        <v>96</v>
+      </c>
+      <c r="O12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2016,36 +2086,15 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>106</v>
-      </c>
-      <c r="G13" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="I13" t="s">
-        <v>108</v>
-      </c>
-      <c r="J13" t="s">
-        <v>109</v>
-      </c>
-      <c r="K13" t="s">
-        <v>110</v>
-      </c>
-      <c r="L13" t="s">
-        <v>111</v>
-      </c>
-      <c r="M13" t="s">
-        <v>35</v>
-      </c>
-      <c r="N13" t="s">
-        <v>112</v>
-      </c>
-      <c r="O13" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2058,78 +2107,78 @@
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="G14" t="s">
+        <v>103</v>
+      </c>
+      <c r="I14" t="s">
+        <v>104</v>
+      </c>
+      <c r="J14" t="s">
+        <v>105</v>
+      </c>
+      <c r="K14" t="s">
+        <v>106</v>
+      </c>
+      <c r="L14" t="s">
         <v>107</v>
-      </c>
-      <c r="I14" t="s">
-        <v>108</v>
-      </c>
-      <c r="J14" t="s">
-        <v>109</v>
-      </c>
-      <c r="K14" t="s">
-        <v>110</v>
-      </c>
-      <c r="L14" t="s">
-        <v>111</v>
       </c>
       <c r="M14" t="s">
         <v>35</v>
       </c>
       <c r="N14" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="O14" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
         <v>1</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="G15" t="s">
+        <v>103</v>
+      </c>
+      <c r="I15" t="s">
+        <v>104</v>
+      </c>
+      <c r="J15" t="s">
+        <v>105</v>
+      </c>
+      <c r="K15" t="s">
+        <v>106</v>
+      </c>
+      <c r="L15" t="s">
         <v>107</v>
-      </c>
-      <c r="H15" t="s">
-        <v>118</v>
-      </c>
-      <c r="I15" t="s">
-        <v>108</v>
-      </c>
-      <c r="J15" t="s">
-        <v>109</v>
-      </c>
-      <c r="K15" t="s">
-        <v>110</v>
-      </c>
-      <c r="L15" t="s">
-        <v>119</v>
       </c>
       <c r="M15" t="s">
         <v>35</v>
       </c>
       <c r="N15" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="O15" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -2139,324 +2188,324 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="G16" t="s">
-        <v>107</v>
+        <v>103</v>
+      </c>
+      <c r="H16" t="s">
+        <v>114</v>
       </c>
       <c r="I16" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="J16" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="K16" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="L16" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="M16" t="s">
         <v>35</v>
       </c>
       <c r="N16" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="O16" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.45">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B17">
-        <v>8</v>
-      </c>
-      <c r="C17">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G17" t="s">
+        <v>103</v>
+      </c>
+      <c r="I17" t="s">
+        <v>104</v>
+      </c>
+      <c r="J17" t="s">
+        <v>105</v>
+      </c>
+      <c r="K17" t="s">
+        <v>106</v>
+      </c>
+      <c r="L17" t="s">
         <v>107</v>
-      </c>
-      <c r="I17" t="s">
-        <v>108</v>
-      </c>
-      <c r="J17" t="s">
-        <v>109</v>
-      </c>
-      <c r="K17" t="s">
-        <v>110</v>
-      </c>
-      <c r="L17" t="s">
-        <v>111</v>
       </c>
       <c r="M17" t="s">
         <v>35</v>
       </c>
       <c r="N17" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="O17" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.45">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="G18" t="s">
+        <v>103</v>
+      </c>
+      <c r="I18" t="s">
+        <v>104</v>
+      </c>
+      <c r="J18" t="s">
+        <v>105</v>
+      </c>
+      <c r="K18" t="s">
+        <v>106</v>
+      </c>
+      <c r="L18" t="s">
         <v>107</v>
-      </c>
-      <c r="I18" t="s">
-        <v>108</v>
-      </c>
-      <c r="J18" t="s">
-        <v>109</v>
-      </c>
-      <c r="K18" t="s">
-        <v>110</v>
-      </c>
-      <c r="L18" t="s">
-        <v>111</v>
       </c>
       <c r="M18" t="s">
         <v>35</v>
       </c>
       <c r="N18" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="O18" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.45">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B19">
-        <v>6</v>
-      </c>
-      <c r="C19">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F19" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="G19" t="s">
+        <v>103</v>
+      </c>
+      <c r="I19" t="s">
+        <v>104</v>
+      </c>
+      <c r="J19" t="s">
+        <v>105</v>
+      </c>
+      <c r="K19" t="s">
+        <v>106</v>
+      </c>
+      <c r="L19" t="s">
         <v>107</v>
-      </c>
-      <c r="I19" t="s">
-        <v>108</v>
-      </c>
-      <c r="J19" t="s">
-        <v>109</v>
-      </c>
-      <c r="K19" t="s">
-        <v>110</v>
-      </c>
-      <c r="L19" t="s">
-        <v>111</v>
       </c>
       <c r="M19" t="s">
         <v>35</v>
       </c>
       <c r="N19" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="O19" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.45">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G20" t="s">
+        <v>103</v>
+      </c>
+      <c r="I20" t="s">
+        <v>104</v>
+      </c>
+      <c r="J20" t="s">
+        <v>105</v>
+      </c>
+      <c r="K20" t="s">
+        <v>106</v>
+      </c>
+      <c r="L20" t="s">
         <v>107</v>
-      </c>
-      <c r="I20" t="s">
-        <v>108</v>
-      </c>
-      <c r="J20" t="s">
-        <v>109</v>
-      </c>
-      <c r="K20" t="s">
-        <v>110</v>
-      </c>
-      <c r="L20" t="s">
-        <v>111</v>
       </c>
       <c r="M20" t="s">
         <v>35</v>
       </c>
       <c r="N20" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="O20" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.45">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="G21" t="s">
+        <v>103</v>
+      </c>
+      <c r="I21" t="s">
+        <v>104</v>
+      </c>
+      <c r="J21" t="s">
+        <v>105</v>
+      </c>
+      <c r="K21" t="s">
+        <v>106</v>
+      </c>
+      <c r="L21" t="s">
         <v>107</v>
-      </c>
-      <c r="I21" t="s">
-        <v>108</v>
-      </c>
-      <c r="J21" t="s">
-        <v>109</v>
-      </c>
-      <c r="K21" t="s">
-        <v>110</v>
-      </c>
-      <c r="L21" t="s">
-        <v>111</v>
       </c>
       <c r="M21" t="s">
         <v>35</v>
       </c>
       <c r="N21" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="O21" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.45">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B22">
         <v>1</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="G22" t="s">
+        <v>103</v>
+      </c>
+      <c r="I22" t="s">
+        <v>104</v>
+      </c>
+      <c r="J22" t="s">
+        <v>105</v>
+      </c>
+      <c r="K22" t="s">
+        <v>106</v>
+      </c>
+      <c r="L22" t="s">
         <v>107</v>
-      </c>
-      <c r="I22" t="s">
-        <v>108</v>
-      </c>
-      <c r="J22" t="s">
-        <v>109</v>
-      </c>
-      <c r="K22" t="s">
-        <v>110</v>
-      </c>
-      <c r="L22" t="s">
-        <v>111</v>
       </c>
       <c r="M22" t="s">
         <v>35</v>
       </c>
       <c r="N22" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="O22" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.45">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23">
         <v>1</v>
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="G23" t="s">
+        <v>103</v>
+      </c>
+      <c r="I23" t="s">
+        <v>104</v>
+      </c>
+      <c r="J23" t="s">
+        <v>105</v>
+      </c>
+      <c r="K23" t="s">
+        <v>106</v>
+      </c>
+      <c r="L23" t="s">
         <v>107</v>
-      </c>
-      <c r="I23" t="s">
-        <v>108</v>
-      </c>
-      <c r="J23" t="s">
-        <v>109</v>
-      </c>
-      <c r="K23" t="s">
-        <v>110</v>
-      </c>
-      <c r="L23" t="s">
-        <v>111</v>
       </c>
       <c r="M23" t="s">
         <v>35</v>
       </c>
       <c r="N23" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="O23" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.45">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -2469,36 +2518,36 @@
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="G24" t="s">
+        <v>103</v>
+      </c>
+      <c r="I24" t="s">
+        <v>104</v>
+      </c>
+      <c r="J24" t="s">
+        <v>105</v>
+      </c>
+      <c r="K24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L24" t="s">
         <v>107</v>
-      </c>
-      <c r="I24" t="s">
-        <v>108</v>
-      </c>
-      <c r="J24" t="s">
-        <v>109</v>
-      </c>
-      <c r="K24" t="s">
-        <v>110</v>
-      </c>
-      <c r="L24" t="s">
-        <v>111</v>
       </c>
       <c r="M24" t="s">
         <v>35</v>
       </c>
       <c r="N24" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="O24" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.45">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -2511,332 +2560,374 @@
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="G25" t="s">
-        <v>141</v>
-      </c>
-      <c r="H25" t="s">
-        <v>142</v>
+        <v>103</v>
       </c>
       <c r="I25" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="J25" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="K25" t="s">
-        <v>144</v>
+        <v>106</v>
       </c>
       <c r="L25" t="s">
-        <v>145</v>
+        <v>107</v>
       </c>
       <c r="M25" t="s">
         <v>35</v>
       </c>
       <c r="N25" t="s">
-        <v>146</v>
+        <v>108</v>
       </c>
       <c r="O25" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.45">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
       </c>
       <c r="E26">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>119</v>
+      </c>
+      <c r="G26" t="s">
+        <v>137</v>
+      </c>
+      <c r="H26" t="s">
+        <v>138</v>
+      </c>
+      <c r="I26" t="s">
+        <v>104</v>
+      </c>
+      <c r="J26" t="s">
+        <v>139</v>
+      </c>
+      <c r="K26" t="s">
+        <v>140</v>
+      </c>
+      <c r="L26" t="s">
+        <v>141</v>
+      </c>
+      <c r="M26" t="s">
+        <v>35</v>
+      </c>
+      <c r="N26" t="s">
+        <v>142</v>
+      </c>
+      <c r="O26" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>208</v>
+      </c>
+      <c r="B27">
         <v>2</v>
-      </c>
-      <c r="F26" t="s">
-        <v>129</v>
-      </c>
-      <c r="G26" t="s">
-        <v>149</v>
-      </c>
-      <c r="I26" t="s">
-        <v>150</v>
-      </c>
-      <c r="J26" t="s">
-        <v>151</v>
-      </c>
-      <c r="K26" t="s">
-        <v>152</v>
-      </c>
-      <c r="L26" t="s">
-        <v>153</v>
-      </c>
-      <c r="M26" t="s">
-        <v>22</v>
-      </c>
-      <c r="N26" t="s">
-        <v>154</v>
-      </c>
-      <c r="O26" t="s">
-        <v>155</v>
-      </c>
-      <c r="P26" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>156</v>
-      </c>
-      <c r="R26" t="s">
-        <v>157</v>
-      </c>
-      <c r="S26" t="s">
-        <v>24</v>
-      </c>
-      <c r="T26" t="s">
-        <v>158</v>
-      </c>
-      <c r="U26" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>160</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
       </c>
       <c r="E27">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G27" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="I27" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="J27" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="K27" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="L27" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="M27" t="s">
         <v>22</v>
       </c>
       <c r="N27" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="O27" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="P27" t="s">
         <v>35</v>
       </c>
       <c r="Q27" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="R27" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="S27" t="s">
         <v>24</v>
       </c>
       <c r="T27" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="U27" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.45">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>162</v>
+        <v>209</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
       <c r="E28">
+        <f>MAX(0,B28-C28-D28)</f>
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>125</v>
+      </c>
+      <c r="G28" t="s">
+        <v>144</v>
+      </c>
+      <c r="I28" t="s">
+        <v>145</v>
+      </c>
+      <c r="J28" t="s">
+        <v>156</v>
+      </c>
+      <c r="K28" t="s">
+        <v>157</v>
+      </c>
+      <c r="L28" t="s">
+        <v>158</v>
+      </c>
+      <c r="M28" t="s">
+        <v>24</v>
+      </c>
+      <c r="N28" t="s">
+        <v>159</v>
+      </c>
+      <c r="O28" t="s">
+        <v>160</v>
+      </c>
+      <c r="P28" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>161</v>
+      </c>
+      <c r="R28" t="s">
+        <v>162</v>
+      </c>
+      <c r="S28" t="s">
+        <v>24</v>
+      </c>
+      <c r="T28" t="s">
+        <v>153</v>
+      </c>
+      <c r="U28" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>210</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
+        <v>125</v>
+      </c>
+      <c r="G29" t="s">
+        <v>155</v>
+      </c>
+      <c r="I29" t="s">
+        <v>145</v>
+      </c>
+      <c r="J29" t="s">
+        <v>146</v>
+      </c>
+      <c r="K29" t="s">
+        <v>147</v>
+      </c>
+      <c r="L29" t="s">
+        <v>148</v>
+      </c>
+      <c r="M29" t="s">
+        <v>22</v>
+      </c>
+      <c r="N29" t="s">
+        <v>149</v>
+      </c>
+      <c r="O29" t="s">
+        <v>150</v>
+      </c>
+      <c r="P29" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>151</v>
+      </c>
+      <c r="R29" t="s">
+        <v>152</v>
+      </c>
+      <c r="S29" t="s">
+        <v>24</v>
+      </c>
+      <c r="T29" t="s">
+        <v>153</v>
+      </c>
+      <c r="U29" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>163</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="E30">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F28" t="s">
-        <v>129</v>
-      </c>
-      <c r="G28" t="s">
-        <v>149</v>
-      </c>
-      <c r="I28" t="s">
-        <v>150</v>
-      </c>
-      <c r="J28" t="s">
-        <v>163</v>
-      </c>
-      <c r="K28" t="s">
+      <c r="F30" t="s">
         <v>164</v>
       </c>
-      <c r="L28" t="s">
+      <c r="I30" t="s">
         <v>165</v>
       </c>
-      <c r="M28" t="s">
-        <v>24</v>
-      </c>
-      <c r="N28" t="s">
+      <c r="J30" t="s">
         <v>166</v>
       </c>
-      <c r="O28" t="s">
+      <c r="K30" t="s">
         <v>167</v>
       </c>
-      <c r="P28" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q28" t="s">
+      <c r="L30" t="s">
         <v>168</v>
       </c>
-      <c r="R28" t="s">
+      <c r="M30" t="s">
+        <v>35</v>
+      </c>
+      <c r="N30" t="s">
         <v>169</v>
       </c>
-      <c r="S28" t="s">
-        <v>24</v>
-      </c>
-      <c r="T28" t="s">
-        <v>158</v>
-      </c>
-      <c r="U28" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
+      <c r="O30" t="s">
         <v>170</v>
       </c>
-      <c r="B29">
-        <v>2</v>
-      </c>
-      <c r="E29">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F29" t="s">
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>171</v>
       </c>
-      <c r="I29" t="s">
-        <v>172</v>
-      </c>
-      <c r="J29" t="s">
-        <v>173</v>
-      </c>
-      <c r="K29" t="s">
-        <v>174</v>
-      </c>
-      <c r="L29" t="s">
-        <v>175</v>
-      </c>
-      <c r="M29" t="s">
-        <v>35</v>
-      </c>
-      <c r="N29" t="s">
-        <v>176</v>
-      </c>
-      <c r="O29" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>178</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="E30">
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="E31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F31" t="s">
+        <v>172</v>
+      </c>
+      <c r="H31" t="s">
+        <v>173</v>
+      </c>
+      <c r="I31" t="s">
+        <v>174</v>
+      </c>
+      <c r="J31" t="s">
+        <v>175</v>
+      </c>
+      <c r="K31" t="s">
+        <v>176</v>
+      </c>
+      <c r="L31" t="s">
+        <v>177</v>
+      </c>
+      <c r="M31" t="s">
+        <v>178</v>
+      </c>
+      <c r="N31" t="s">
         <v>179</v>
       </c>
-      <c r="H30" t="s">
+      <c r="O31" t="s">
         <v>180</v>
       </c>
-      <c r="I30" t="s">
+      <c r="P31" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q31" t="s">
         <v>181</v>
       </c>
-      <c r="J30" t="s">
+      <c r="R31" t="s">
         <v>182</v>
       </c>
-      <c r="K30" t="s">
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>183</v>
       </c>
-      <c r="L30" t="s">
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F32" t="s">
         <v>184</v>
       </c>
-      <c r="M30" t="s">
+      <c r="I32" t="s">
         <v>185</v>
       </c>
-      <c r="N30" t="s">
+      <c r="J32" t="s">
         <v>186</v>
       </c>
-      <c r="O30" t="s">
+      <c r="K32" t="s">
         <v>187</v>
       </c>
-      <c r="P30" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q30" t="s">
+      <c r="L32" t="s">
         <v>188</v>
       </c>
-      <c r="R30" t="s">
+      <c r="M32" t="s">
+        <v>35</v>
+      </c>
+      <c r="N32" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
+      <c r="O32" t="s">
         <v>190</v>
       </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="E31">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F31" t="s">
-        <v>191</v>
-      </c>
-      <c r="I31" t="s">
-        <v>192</v>
-      </c>
-      <c r="J31" t="s">
-        <v>193</v>
-      </c>
-      <c r="K31" t="s">
-        <v>194</v>
-      </c>
-      <c r="L31" t="s">
-        <v>195</v>
-      </c>
-      <c r="M31" t="s">
-        <v>35</v>
-      </c>
-      <c r="N31" t="s">
-        <v>196</v>
-      </c>
-      <c r="O31" t="s">
-        <v>197</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E31">
+  <conditionalFormatting sqref="E2:E32">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
VCF-4P: BOM - wip
</commit_message>
<xml_diff>
--- a/modules/VCF-4P/VCF-4P-BOM.xlsx
+++ b/modules/VCF-4P/VCF-4P-BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Len\Documents\Dev\git\Synth-priv\modules\VCF-4P\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\VCF-4P\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240497DD-DE7A-443A-9379-AA281757193A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AF813A-F95B-45CF-AD7C-A57B104B2DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="885" yWindow="2145" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VCF-4P-BOM" sheetId="1" r:id="rId1"/>
@@ -1519,16 +1519,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="5" width="4.3984375" customWidth="1"/>
+    <col min="2" max="5" width="4.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1593,7 +1594,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1635,7 +1636,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1677,7 +1678,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1719,7 +1720,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -1761,7 +1762,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -1803,7 +1804,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>194</v>
       </c>
@@ -1845,7 +1846,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>195</v>
       </c>
@@ -1896,7 +1897,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>205</v>
       </c>
@@ -1917,7 +1918,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>206</v>
       </c>
@@ -1965,7 +1966,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>207</v>
       </c>
@@ -2022,7 +2023,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>91</v>
       </c>
@@ -2061,7 +2062,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>98</v>
       </c>
@@ -2082,7 +2083,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>101</v>
       </c>
@@ -2124,7 +2125,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>110</v>
       </c>
@@ -2166,7 +2167,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>112</v>
       </c>
@@ -2208,7 +2209,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>118</v>
       </c>
@@ -2247,7 +2248,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>120</v>
       </c>
@@ -2289,7 +2290,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>122</v>
       </c>
@@ -2328,7 +2329,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>124</v>
       </c>
@@ -2370,7 +2371,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>126</v>
       </c>
@@ -2412,7 +2413,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>128</v>
       </c>
@@ -2454,7 +2455,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>130</v>
       </c>
@@ -2493,7 +2494,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>132</v>
       </c>
@@ -2535,7 +2536,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>134</v>
       </c>
@@ -2577,7 +2578,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>136</v>
       </c>
@@ -2622,7 +2623,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>208</v>
       </c>
@@ -2682,7 +2683,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>209</v>
       </c>
@@ -2742,7 +2743,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>210</v>
       </c>
@@ -2802,7 +2803,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>163</v>
       </c>
@@ -2841,7 +2842,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>171</v>
       </c>
@@ -2892,7 +2893,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>183</v>
       </c>

</xml_diff>

<commit_message>
VCF-4P: - adjust a resistor - update BOM
</commit_message>
<xml_diff>
--- a/modules/VCF-4P/VCF-4P-BOM.xlsx
+++ b/modules/VCF-4P/VCF-4P-BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\VCF-4P\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6A8E95-4068-4341-A819-66AAF1DA26F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BF889D-BC87-49C2-8ED9-5861741A64B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4935" yWindow="1275" windowWidth="19395" windowHeight="11685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7560" yWindow="2505" windowWidth="19395" windowHeight="11685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VCF-4P-BOM" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="250">
   <si>
     <t>Ref</t>
   </si>
@@ -430,9 +430,6 @@
     <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-12FTF52-36K?qs=oAGoVhmvjhyIq6EO5blb%252BQ%3D%3D</t>
   </si>
   <si>
-    <t>R3 R23</t>
-  </si>
-  <si>
     <t>30K</t>
   </si>
   <si>
@@ -770,6 +767,21 @@
   </si>
   <si>
     <t>DAB2140</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>24K</t>
+  </si>
+  <si>
+    <t>MFR-12FTF52-24K</t>
+  </si>
+  <si>
+    <t>603-MFR-12FTF52-24K</t>
   </si>
 </sst>
 </file>
@@ -1633,10 +1645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U33"/>
+  <dimension ref="A1:U34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1652,13 +1664,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>242</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -1762,7 +1774,7 @@
         <v>2</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E33" si="0">MAX(0,B3-C3-D3)</f>
+        <f t="shared" ref="E3:E34" si="0">MAX(0,B3-C3-D3)</f>
         <v>0</v>
       </c>
       <c r="F3" t="s">
@@ -1859,7 +1871,7 @@
         <v>29</v>
       </c>
       <c r="H5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I5" t="s">
         <v>49</v>
@@ -2341,20 +2353,20 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>132</v>
+        <v>246</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>133</v>
+        <v>247</v>
       </c>
       <c r="G17" t="s">
         <v>120</v>
@@ -2369,21 +2381,19 @@
         <v>123</v>
       </c>
       <c r="L17" t="s">
-        <v>134</v>
+        <v>248</v>
       </c>
       <c r="M17" t="s">
         <v>35</v>
       </c>
       <c r="N17" t="s">
-        <v>135</v>
-      </c>
-      <c r="O17" t="s">
-        <v>136</v>
-      </c>
+        <v>249</v>
+      </c>
+      <c r="O17" s="2"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -2393,7 +2403,7 @@
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G18" t="s">
         <v>120</v>
@@ -2408,21 +2418,21 @@
         <v>123</v>
       </c>
       <c r="L18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M18" t="s">
         <v>35</v>
       </c>
       <c r="N18" t="s">
+        <v>139</v>
+      </c>
+      <c r="O18" t="s">
         <v>140</v>
-      </c>
-      <c r="O18" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B19">
         <v>8</v>
@@ -2435,7 +2445,7 @@
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G19" t="s">
         <v>120</v>
@@ -2450,31 +2460,34 @@
         <v>123</v>
       </c>
       <c r="L19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="M19" t="s">
         <v>35</v>
       </c>
       <c r="N19" t="s">
+        <v>144</v>
+      </c>
+      <c r="O19" t="s">
         <v>145</v>
-      </c>
-      <c r="O19" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B20">
         <v>4</v>
       </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G20" t="s">
         <v>120</v>
@@ -2489,21 +2502,21 @@
         <v>123</v>
       </c>
       <c r="L20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M20" t="s">
         <v>35</v>
       </c>
       <c r="N20" t="s">
+        <v>149</v>
+      </c>
+      <c r="O20" t="s">
         <v>150</v>
-      </c>
-      <c r="O20" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -2513,7 +2526,7 @@
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G21" t="s">
         <v>120</v>
@@ -2528,21 +2541,21 @@
         <v>123</v>
       </c>
       <c r="L21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M21" t="s">
         <v>35</v>
       </c>
       <c r="N21" t="s">
+        <v>154</v>
+      </c>
+      <c r="O21" t="s">
         <v>155</v>
-      </c>
-      <c r="O21" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -2555,7 +2568,7 @@
         <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G22" t="s">
         <v>120</v>
@@ -2570,21 +2583,21 @@
         <v>123</v>
       </c>
       <c r="L22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M22" t="s">
         <v>35</v>
       </c>
       <c r="N22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="O22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -2597,7 +2610,7 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G23" t="s">
         <v>120</v>
@@ -2612,34 +2625,34 @@
         <v>123</v>
       </c>
       <c r="L23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M23" t="s">
         <v>35</v>
       </c>
       <c r="N23" t="s">
+        <v>163</v>
+      </c>
+      <c r="O23" t="s">
         <v>164</v>
-      </c>
-      <c r="O23" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>166</v>
+        <v>245</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E24" si="1">MAX(0,B24-C24-D24)</f>
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
       <c r="G24" t="s">
         <v>120</v>
@@ -2654,66 +2667,63 @@
         <v>123</v>
       </c>
       <c r="L24" t="s">
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="M24" t="s">
         <v>35</v>
       </c>
       <c r="N24" t="s">
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="O24" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="G25" t="s">
-        <v>172</v>
-      </c>
-      <c r="H25" t="s">
-        <v>173</v>
+        <v>120</v>
       </c>
       <c r="I25" t="s">
         <v>121</v>
       </c>
       <c r="J25" t="s">
-        <v>174</v>
+        <v>122</v>
       </c>
       <c r="K25" t="s">
-        <v>175</v>
+        <v>123</v>
       </c>
       <c r="L25" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="M25" t="s">
         <v>35</v>
       </c>
       <c r="N25" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="O25" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -2726,36 +2736,39 @@
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>180</v>
+        <v>137</v>
       </c>
       <c r="G26" t="s">
-        <v>120</v>
+        <v>171</v>
       </c>
       <c r="H26" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="I26" t="s">
         <v>121</v>
       </c>
       <c r="J26" t="s">
-        <v>122</v>
+        <v>173</v>
       </c>
       <c r="K26" t="s">
-        <v>123</v>
+        <v>174</v>
       </c>
       <c r="L26" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="M26" t="s">
         <v>35</v>
       </c>
+      <c r="N26" t="s">
+        <v>176</v>
+      </c>
       <c r="O26" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -2768,60 +2781,42 @@
         <v>0</v>
       </c>
       <c r="F27" t="s">
-        <v>119</v>
+        <v>179</v>
       </c>
       <c r="G27" t="s">
-        <v>185</v>
+        <v>120</v>
+      </c>
+      <c r="H27" t="s">
+        <v>180</v>
       </c>
       <c r="I27" t="s">
-        <v>186</v>
+        <v>121</v>
       </c>
       <c r="J27" t="s">
-        <v>187</v>
+        <v>122</v>
       </c>
       <c r="K27" t="s">
-        <v>188</v>
+        <v>123</v>
       </c>
       <c r="L27" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="M27" t="s">
-        <v>22</v>
-      </c>
-      <c r="N27" t="s">
-        <v>190</v>
+        <v>35</v>
       </c>
       <c r="O27" t="s">
-        <v>191</v>
-      </c>
-      <c r="P27" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>192</v>
-      </c>
-      <c r="R27" t="s">
-        <v>193</v>
-      </c>
-      <c r="S27" t="s">
-        <v>24</v>
-      </c>
-      <c r="T27" t="s">
-        <v>194</v>
-      </c>
-      <c r="U27" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="B28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28">
         <f t="shared" si="0"/>
@@ -2831,57 +2826,57 @@
         <v>119</v>
       </c>
       <c r="G28" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="I28" t="s">
+        <v>185</v>
+      </c>
+      <c r="J28" t="s">
         <v>186</v>
       </c>
-      <c r="J28" t="s">
-        <v>198</v>
-      </c>
       <c r="K28" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="L28" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="M28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="N28" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="O28" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="P28" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="Q28" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="R28" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="S28" t="s">
         <v>24</v>
       </c>
       <c r="T28" t="s">
+        <v>193</v>
+      </c>
+      <c r="U28" t="s">
         <v>194</v>
-      </c>
-      <c r="U28" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E29">
         <f t="shared" si="0"/>
@@ -2891,144 +2886,147 @@
         <v>119</v>
       </c>
       <c r="G29" t="s">
+        <v>196</v>
+      </c>
+      <c r="I29" t="s">
+        <v>185</v>
+      </c>
+      <c r="J29" t="s">
         <v>197</v>
       </c>
-      <c r="I29" t="s">
-        <v>186</v>
-      </c>
-      <c r="J29" t="s">
-        <v>187</v>
-      </c>
       <c r="K29" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="L29" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="M29" t="s">
+        <v>24</v>
+      </c>
+      <c r="N29" t="s">
+        <v>200</v>
+      </c>
+      <c r="O29" t="s">
+        <v>201</v>
+      </c>
+      <c r="P29" t="s">
         <v>22</v>
       </c>
-      <c r="N29" t="s">
-        <v>190</v>
-      </c>
-      <c r="O29" t="s">
-        <v>191</v>
-      </c>
-      <c r="P29" t="s">
-        <v>35</v>
-      </c>
       <c r="Q29" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="R29" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="S29" t="s">
         <v>24</v>
       </c>
       <c r="T29" t="s">
+        <v>193</v>
+      </c>
+      <c r="U29" t="s">
         <v>194</v>
-      </c>
-      <c r="U29" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B30">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
       </c>
       <c r="E30">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F30" t="s">
-        <v>143</v>
+        <v>119</v>
+      </c>
+      <c r="G30" t="s">
+        <v>196</v>
       </c>
       <c r="I30" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="J30" t="s">
-        <v>208</v>
+        <v>186</v>
       </c>
       <c r="K30" t="s">
-        <v>209</v>
+        <v>187</v>
       </c>
       <c r="L30" t="s">
-        <v>210</v>
+        <v>188</v>
       </c>
       <c r="M30" t="s">
+        <v>22</v>
+      </c>
+      <c r="N30" t="s">
+        <v>189</v>
+      </c>
+      <c r="O30" t="s">
+        <v>190</v>
+      </c>
+      <c r="P30" t="s">
         <v>35</v>
       </c>
-      <c r="N30" t="s">
-        <v>211</v>
-      </c>
-      <c r="O30" t="s">
-        <v>212</v>
+      <c r="Q30" t="s">
+        <v>191</v>
+      </c>
+      <c r="R30" t="s">
+        <v>192</v>
+      </c>
+      <c r="S30" t="s">
+        <v>24</v>
+      </c>
+      <c r="T30" t="s">
+        <v>193</v>
+      </c>
+      <c r="U30" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E31">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F31" t="s">
-        <v>214</v>
-      </c>
-      <c r="H31" t="s">
-        <v>215</v>
+        <v>142</v>
       </c>
       <c r="I31" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="J31" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="K31" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="L31" t="s">
-        <v>245</v>
+        <v>209</v>
       </c>
       <c r="M31" t="s">
-        <v>219</v>
+        <v>35</v>
       </c>
       <c r="N31" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="O31" t="s">
-        <v>221</v>
-      </c>
-      <c r="P31" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>222</v>
-      </c>
-      <c r="R31" t="s">
-        <v>223</v>
-      </c>
-      <c r="S31" t="s">
-        <v>22</v>
-      </c>
-      <c r="U31" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -3041,33 +3039,51 @@
         <v>0</v>
       </c>
       <c r="F32" t="s">
-        <v>226</v>
+        <v>213</v>
+      </c>
+      <c r="H32" t="s">
+        <v>214</v>
       </c>
       <c r="I32" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="J32" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="K32" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="L32" t="s">
-        <v>230</v>
+        <v>244</v>
       </c>
       <c r="M32" t="s">
-        <v>35</v>
+        <v>218</v>
       </c>
       <c r="N32" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="O32" t="s">
-        <v>232</v>
+        <v>220</v>
+      </c>
+      <c r="P32" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>221</v>
+      </c>
+      <c r="R32" t="s">
+        <v>222</v>
+      </c>
+      <c r="S32" t="s">
+        <v>22</v>
+      </c>
+      <c r="U32" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -3080,32 +3096,71 @@
         <v>0</v>
       </c>
       <c r="F33" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="I33" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="J33" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="K33" t="s">
+        <v>228</v>
+      </c>
+      <c r="L33" t="s">
         <v>229</v>
-      </c>
-      <c r="L33" t="s">
-        <v>237</v>
       </c>
       <c r="M33" t="s">
         <v>35</v>
       </c>
       <c r="N33" t="s">
+        <v>230</v>
+      </c>
+      <c r="O33" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>232</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>233</v>
+      </c>
+      <c r="I34" t="s">
+        <v>234</v>
+      </c>
+      <c r="J34" t="s">
+        <v>235</v>
+      </c>
+      <c r="K34" t="s">
+        <v>228</v>
+      </c>
+      <c r="L34" t="s">
+        <v>236</v>
+      </c>
+      <c r="M34" t="s">
+        <v>35</v>
+      </c>
+      <c r="N34" t="s">
+        <v>237</v>
+      </c>
+      <c r="O34" t="s">
         <v>238</v>
       </c>
-      <c r="O33" t="s">
-        <v>239</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E33">
+  <conditionalFormatting sqref="E2:E34">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>